<commit_message>
HTML & CSS Formatting and the resolution bug is fixed
</commit_message>
<xml_diff>
--- a/assets/Testing/Rev02_Testcases.xlsx
+++ b/assets/Testing/Rev02_Testcases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="132" windowWidth="14664" windowHeight="8232" activeTab="2"/>
+    <workbookView xWindow="192" yWindow="132" windowWidth="14664" windowHeight="8232"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="174">
   <si>
     <t>No.</t>
   </si>
@@ -316,9 +316,6 @@
 5. Every icon works on every page</t>
   </si>
   <si>
-    <t>Device 3, Device 4 Horizotal mode : indeximg problem</t>
-  </si>
-  <si>
     <t>Model Name</t>
   </si>
   <si>
@@ -449,9 +446,6 @@
   </si>
   <si>
     <t>Tester Confirm</t>
-  </si>
-  <si>
-    <t>New</t>
   </si>
   <si>
     <t>B</t>
@@ -477,9 +471,6 @@
   </si>
   <si>
     <t>The image ratio is always same.</t>
-  </si>
-  <si>
-    <t>Refer [bugs capture] sheet : Cap1, Cap2</t>
   </si>
   <si>
     <t>Cap 1 : On iPhone Xs Max</t>
@@ -565,13 +556,29 @@
     <t>iPhone XS MAX</t>
   </si>
   <si>
-    <t>Refer [bugs capture] sheet : Cap1</t>
-  </si>
-  <si>
     <t>2020.03.26</t>
   </si>
   <si>
     <t>cf. V30S</t>
+  </si>
+  <si>
+    <t>Closed
+Date</t>
+  </si>
+  <si>
+    <t>2020.03.27</t>
+  </si>
+  <si>
+    <t>The image had a fixed width and height, so the developer gave a responsive ratio on the image.</t>
+  </si>
+  <si>
+    <t>indeximg bug is fixed, please refer the [Bug report] sheet.</t>
+  </si>
+  <si>
+    <t>Refer [Bugs capture] sheet : Cap1, Cap2</t>
+  </si>
+  <si>
+    <t>Refer [Bugs capture] sheet : Cap1</t>
   </si>
 </sst>
 </file>
@@ -650,7 +657,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -677,12 +684,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -690,6 +691,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEBFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1287,7 +1300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1345,9 +1358,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1375,27 +1385,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1405,8 +1397,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1417,52 +1412,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1492,17 +1487,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1539,6 +1549,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFEBFF"/>
       <color rgb="FF008000"/>
     </mruColors>
   </colors>
@@ -1913,11 +1924,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:N57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F54" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1941,96 +1952,96 @@
       <c r="J1" s="12"/>
     </row>
     <row r="2" spans="2:14" ht="18">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="47" t="s">
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="51" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15.6">
-      <c r="B3" s="57"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="59" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="61" t="s">
+      <c r="I3" s="50"/>
+      <c r="J3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="61" t="s">
+      <c r="K3" s="50"/>
+      <c r="L3" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="M3" s="62"/>
-      <c r="N3" s="48"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="52"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B4" s="58"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="43" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="L4" s="43" t="s">
+      <c r="L4" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="M4" s="43" t="s">
+      <c r="M4" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="N4" s="49"/>
+      <c r="N4" s="53"/>
     </row>
     <row r="5" spans="2:14" ht="43.8" thickTop="1">
       <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>148</v>
+      <c r="C5" s="33" t="s">
+        <v>145</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>58</v>
@@ -2062,14 +2073,14 @@
       <c r="B6" s="7">
         <v>2</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="34" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>59</v>
@@ -2101,14 +2112,14 @@
       <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="44" t="s">
-        <v>150</v>
+      <c r="C7" s="38" t="s">
+        <v>147</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>58</v>
@@ -2140,7 +2151,7 @@
       <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="45"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
@@ -2172,19 +2183,19 @@
         <v>58</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="28.8">
       <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="45"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>58</v>
@@ -2216,9 +2227,9 @@
       <c r="B10" s="7">
         <v>6</v>
       </c>
-      <c r="C10" s="45"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>23</v>
@@ -2253,9 +2264,9 @@
       <c r="B11" s="7">
         <v>7</v>
       </c>
-      <c r="C11" s="45"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>24</v>
@@ -2290,9 +2301,9 @@
       <c r="B12" s="7">
         <v>8</v>
       </c>
-      <c r="C12" s="45"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>25</v>
@@ -2327,7 +2338,7 @@
       <c r="B13" s="7">
         <v>9</v>
       </c>
-      <c r="C13" s="45"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="5" t="s">
         <v>16</v>
       </c>
@@ -2364,12 +2375,12 @@
       <c r="B14" s="7">
         <v>10</v>
       </c>
-      <c r="C14" s="45"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>58</v>
@@ -2401,9 +2412,9 @@
       <c r="B15" s="7">
         <v>11</v>
       </c>
-      <c r="C15" s="45"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>27</v>
@@ -2438,7 +2449,7 @@
       <c r="B16" s="7">
         <v>12</v>
       </c>
-      <c r="C16" s="45"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
@@ -2475,7 +2486,7 @@
       <c r="B17" s="7">
         <v>13</v>
       </c>
-      <c r="C17" s="45"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="5" t="s">
         <v>19</v>
       </c>
@@ -2512,12 +2523,12 @@
       <c r="B18" s="7">
         <v>14</v>
       </c>
-      <c r="C18" s="45"/>
+      <c r="C18" s="39"/>
       <c r="D18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>58</v>
@@ -2549,7 +2560,7 @@
       <c r="B19" s="7">
         <v>15</v>
       </c>
-      <c r="C19" s="45"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="5" t="s">
         <v>21</v>
       </c>
@@ -2586,7 +2597,7 @@
       <c r="B20" s="7">
         <v>16</v>
       </c>
-      <c r="C20" s="46"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="5" t="s">
         <v>22</v>
       </c>
@@ -2623,8 +2634,8 @@
       <c r="B21" s="7">
         <v>17</v>
       </c>
-      <c r="C21" s="44" t="s">
-        <v>163</v>
+      <c r="C21" s="38" t="s">
+        <v>160</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>39</v>
@@ -2662,7 +2673,7 @@
       <c r="B22" s="7">
         <v>18</v>
       </c>
-      <c r="C22" s="45"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="5" t="s">
         <v>35</v>
       </c>
@@ -2699,7 +2710,7 @@
       <c r="B23" s="7">
         <v>19</v>
       </c>
-      <c r="C23" s="45"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="5" t="s">
         <v>33</v>
       </c>
@@ -2736,7 +2747,7 @@
       <c r="B24" s="7">
         <v>20</v>
       </c>
-      <c r="C24" s="45"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="5" t="s">
         <v>34</v>
       </c>
@@ -2773,8 +2784,8 @@
       <c r="B25" s="7">
         <v>21</v>
       </c>
-      <c r="C25" s="44" t="s">
-        <v>164</v>
+      <c r="C25" s="38" t="s">
+        <v>161</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>39</v>
@@ -2812,7 +2823,7 @@
       <c r="B26" s="7">
         <v>22</v>
       </c>
-      <c r="C26" s="45"/>
+      <c r="C26" s="39"/>
       <c r="D26" s="5" t="s">
         <v>35</v>
       </c>
@@ -2849,7 +2860,7 @@
       <c r="B27" s="7">
         <v>23</v>
       </c>
-      <c r="C27" s="45"/>
+      <c r="C27" s="39"/>
       <c r="D27" s="5" t="s">
         <v>36</v>
       </c>
@@ -2886,7 +2897,7 @@
       <c r="B28" s="7">
         <v>24</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="38" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -2925,7 +2936,7 @@
       <c r="B29" s="7">
         <v>25</v>
       </c>
-      <c r="C29" s="45"/>
+      <c r="C29" s="39"/>
       <c r="D29" s="5" t="s">
         <v>35</v>
       </c>
@@ -2962,7 +2973,7 @@
       <c r="B30" s="7">
         <v>26</v>
       </c>
-      <c r="C30" s="45"/>
+      <c r="C30" s="39"/>
       <c r="D30" s="5" t="s">
         <v>36</v>
       </c>
@@ -2999,7 +3010,7 @@
       <c r="B31" s="7">
         <v>27</v>
       </c>
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D31" s="5" t="s">
@@ -3038,7 +3049,7 @@
       <c r="B32" s="7">
         <v>28</v>
       </c>
-      <c r="C32" s="45"/>
+      <c r="C32" s="39"/>
       <c r="D32" s="5" t="s">
         <v>35</v>
       </c>
@@ -3075,7 +3086,7 @@
       <c r="B33" s="7">
         <v>29</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="38" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="5" t="s">
@@ -3114,7 +3125,7 @@
       <c r="B34" s="7">
         <v>30</v>
       </c>
-      <c r="C34" s="45"/>
+      <c r="C34" s="39"/>
       <c r="D34" s="5" t="s">
         <v>74</v>
       </c>
@@ -3151,7 +3162,7 @@
       <c r="B35" s="7">
         <v>31</v>
       </c>
-      <c r="C35" s="46"/>
+      <c r="C35" s="40"/>
       <c r="D35" s="5" t="s">
         <v>35</v>
       </c>
@@ -3188,7 +3199,7 @@
       <c r="B36" s="7">
         <v>32</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="38" t="s">
         <v>45</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -3227,7 +3238,7 @@
       <c r="B37" s="7">
         <v>33</v>
       </c>
-      <c r="C37" s="45"/>
+      <c r="C37" s="39"/>
       <c r="D37" s="5" t="s">
         <v>43</v>
       </c>
@@ -3264,7 +3275,7 @@
       <c r="B38" s="7">
         <v>34</v>
       </c>
-      <c r="C38" s="45"/>
+      <c r="C38" s="39"/>
       <c r="D38" s="5" t="s">
         <v>35</v>
       </c>
@@ -3301,7 +3312,7 @@
       <c r="B39" s="7">
         <v>35</v>
       </c>
-      <c r="C39" s="46"/>
+      <c r="C39" s="40"/>
       <c r="D39" s="5" t="s">
         <v>47</v>
       </c>
@@ -3338,7 +3349,7 @@
       <c r="B40" s="7">
         <v>36</v>
       </c>
-      <c r="C40" s="44" t="s">
+      <c r="C40" s="38" t="s">
         <v>48</v>
       </c>
       <c r="D40" s="5" t="s">
@@ -3377,7 +3388,7 @@
       <c r="B41" s="7">
         <v>37</v>
       </c>
-      <c r="C41" s="45"/>
+      <c r="C41" s="39"/>
       <c r="D41" s="5" t="s">
         <v>43</v>
       </c>
@@ -3414,7 +3425,7 @@
       <c r="B42" s="7">
         <v>38</v>
       </c>
-      <c r="C42" s="45"/>
+      <c r="C42" s="39"/>
       <c r="D42" s="5" t="s">
         <v>35</v>
       </c>
@@ -3451,7 +3462,7 @@
       <c r="B43" s="7">
         <v>39</v>
       </c>
-      <c r="C43" s="46"/>
+      <c r="C43" s="40"/>
       <c r="D43" s="5" t="s">
         <v>47</v>
       </c>
@@ -3488,7 +3499,7 @@
       <c r="B44" s="7">
         <v>40</v>
       </c>
-      <c r="C44" s="44" t="s">
+      <c r="C44" s="38" t="s">
         <v>52</v>
       </c>
       <c r="D44" s="5" t="s">
@@ -3527,7 +3538,7 @@
       <c r="B45" s="7">
         <v>41</v>
       </c>
-      <c r="C45" s="45"/>
+      <c r="C45" s="39"/>
       <c r="D45" s="5" t="s">
         <v>35</v>
       </c>
@@ -3564,7 +3575,7 @@
       <c r="B46" s="7">
         <v>42</v>
       </c>
-      <c r="C46" s="45"/>
+      <c r="C46" s="39"/>
       <c r="D46" s="5" t="s">
         <v>53</v>
       </c>
@@ -3601,7 +3612,7 @@
       <c r="B47" s="7">
         <v>43</v>
       </c>
-      <c r="C47" s="46"/>
+      <c r="C47" s="40"/>
       <c r="D47" s="5" t="s">
         <v>54</v>
       </c>
@@ -3638,7 +3649,7 @@
       <c r="B48" s="7">
         <v>44</v>
       </c>
-      <c r="C48" s="44" t="s">
+      <c r="C48" s="38" t="s">
         <v>55</v>
       </c>
       <c r="D48" s="5" t="s">
@@ -3677,7 +3688,7 @@
       <c r="B49" s="7">
         <v>45</v>
       </c>
-      <c r="C49" s="45"/>
+      <c r="C49" s="39"/>
       <c r="D49" s="5" t="s">
         <v>35</v>
       </c>
@@ -3714,7 +3725,7 @@
       <c r="B50" s="7">
         <v>46</v>
       </c>
-      <c r="C50" s="45"/>
+      <c r="C50" s="39"/>
       <c r="D50" s="5" t="s">
         <v>53</v>
       </c>
@@ -3751,7 +3762,7 @@
       <c r="B51" s="7">
         <v>47</v>
       </c>
-      <c r="C51" s="46"/>
+      <c r="C51" s="40"/>
       <c r="D51" s="5" t="s">
         <v>54</v>
       </c>
@@ -3788,7 +3799,7 @@
       <c r="B52" s="7">
         <v>48</v>
       </c>
-      <c r="C52" s="44" t="s">
+      <c r="C52" s="38" t="s">
         <v>56</v>
       </c>
       <c r="D52" s="5" t="s">
@@ -3827,7 +3838,7 @@
       <c r="B53" s="7">
         <v>49</v>
       </c>
-      <c r="C53" s="45"/>
+      <c r="C53" s="39"/>
       <c r="D53" s="5" t="s">
         <v>81</v>
       </c>
@@ -3864,7 +3875,7 @@
       <c r="B54" s="7">
         <v>50</v>
       </c>
-      <c r="C54" s="45"/>
+      <c r="C54" s="39"/>
       <c r="D54" s="5" t="s">
         <v>83</v>
       </c>
@@ -3901,7 +3912,7 @@
       <c r="B55" s="7">
         <v>51</v>
       </c>
-      <c r="C55" s="45"/>
+      <c r="C55" s="39"/>
       <c r="D55" s="5" t="s">
         <v>85</v>
       </c>
@@ -3938,7 +3949,7 @@
       <c r="B56" s="7">
         <v>52</v>
       </c>
-      <c r="C56" s="46"/>
+      <c r="C56" s="40"/>
       <c r="D56" s="5" t="s">
         <v>87</v>
       </c>
@@ -3975,7 +3986,7 @@
       <c r="B57" s="8">
         <v>53</v>
       </c>
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="35" t="s">
         <v>32</v>
       </c>
       <c r="D57" s="6" t="s">
@@ -4012,6 +4023,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C7:C20"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="C52:C56"/>
     <mergeCell ref="C21:C24"/>
     <mergeCell ref="C25:C27"/>
@@ -4022,18 +4045,6 @@
     <mergeCell ref="C40:C43"/>
     <mergeCell ref="C44:C47"/>
     <mergeCell ref="C48:C51"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="C7:C20"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="F2:M2"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:M57">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -4053,7 +4064,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:P3"/>
+  <dimension ref="B1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -4071,147 +4082,160 @@
     <col min="10" max="10" width="32.77734375" customWidth="1"/>
     <col min="11" max="11" width="25.88671875" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="13" max="14" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="21.77734375" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="22" customFormat="1" ht="35.4" thickBot="1">
+    <row r="1" spans="2:17" s="22" customFormat="1" ht="35.4" thickBot="1">
       <c r="B1" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="P1" s="21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="2:16" ht="47.4" thickBot="1">
+    </row>
+    <row r="2" spans="2:17" ht="47.4" thickBot="1">
       <c r="B2" s="15">
         <v>1</v>
       </c>
-      <c r="C2" s="75" t="s">
-        <v>167</v>
+      <c r="C2" s="37" t="s">
+        <v>164</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="M2" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="I2" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>137</v>
+      <c r="O2" s="19" t="s">
+        <v>163</v>
       </c>
       <c r="P2" s="16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" ht="47.4" thickBot="1">
+        <v>135</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" ht="78.599999999999994" thickBot="1">
       <c r="B3" s="15">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="L3" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="K3" s="19" t="s">
+      <c r="M3" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="N3" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L3" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="M3" s="17" t="s">
+      <c r="O3" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="P3" s="16"/>
+      <c r="P3" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>135</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4223,18 +4247,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -4245,262 +4269,264 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="25.77734375" style="31" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" style="32" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="30" customWidth="1"/>
+    <col min="3" max="6" width="25.77734375" style="30" customWidth="1"/>
+    <col min="7" max="7" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" thickTop="1">
+    <row r="1" spans="1:7" ht="24" thickTop="1">
       <c r="A1"/>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2"/>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="68"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="62"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3"/>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="68"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="62"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4"/>
-      <c r="B4" s="66" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="68"/>
+      <c r="B4" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="62"/>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:6" ht="15.6">
+    <row r="5" spans="1:7" ht="15.6">
       <c r="A5"/>
-      <c r="B5" s="72" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="74"/>
+      <c r="B5" s="66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="68"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6"/>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="68"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="62"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7"/>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="68"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="62"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8"/>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="68"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9"/>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="68"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="62"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1">
+    <row r="10" spans="1:7" ht="15" thickBot="1">
       <c r="A10"/>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="71"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:6" ht="15.6" thickTop="1" thickBot="1">
+    <row r="11" spans="1:7" ht="15.6" thickTop="1" thickBot="1">
       <c r="A11"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:6" s="12" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A12" s="32"/>
-      <c r="B12" s="37" t="s">
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B12" s="31"/>
+      <c r="C12" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="D12" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="E12" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="F12" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="G12" s="71" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" thickTop="1">
-      <c r="A13" s="33" t="s">
+    <row r="13" spans="1:7" ht="30" customHeight="1" thickTop="1">
+      <c r="B13" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1">
+      <c r="B14" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="C14" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" customHeight="1">
+      <c r="B15" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" customHeight="1">
+      <c r="B16" s="73" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="26" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8">
-      <c r="A14" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F14" s="28" t="s">
+      <c r="G16" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1">
+      <c r="B17" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.8">
-      <c r="A15" s="34" t="s">
+      <c r="F17" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" thickBot="1">
+      <c r="B18" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="27" t="s">
+      <c r="C18" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1">
-      <c r="A18" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>108</v>
+      <c r="F18" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -4517,5 +4543,6 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>